<commit_message>
Exportar documento Productividad: Funciona
</commit_message>
<xml_diff>
--- a/productos_ciclos.xlsx
+++ b/productos_ciclos.xlsx
@@ -340,6 +340,44 @@
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="TablaCiclos_Tarta_de_zanahoria" displayName="TablaCiclos_Tarta_de_zanahoria" ref="A101:J102" headerRowCount="1">
   <autoFilter ref="A101:J102"/>
+  <tableColumns count="10">
+    <tableColumn id="1" name="IdCiclo"/>
+    <tableColumn id="2" name="IdTorre"/>
+    <tableColumn id="3" name="FechaInicio"/>
+    <tableColumn id="4" name="FechaFin"/>
+    <tableColumn id="5" name="TipoFin"/>
+    <tableColumn id="6" name="CantidadNivelesCorrectos"/>
+    <tableColumn id="7" name="PesoTorreFila"/>
+    <tableColumn id="8" name="PesoTorreProducto"/>
+    <tableColumn id="9" name="Lote"/>
+    <tableColumn id="10" name="TiempoTotal"/>
+  </tableColumns>
+  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="TablaCiclos_Tarta_de_mousse_de_fresa" displayName="TablaCiclos_Tarta_de_mousse_de_fresa" ref="A107:J108" headerRowCount="1">
+  <autoFilter ref="A107:J108"/>
+  <tableColumns count="10">
+    <tableColumn id="1" name="IdCiclo"/>
+    <tableColumn id="2" name="IdTorre"/>
+    <tableColumn id="3" name="FechaInicio"/>
+    <tableColumn id="4" name="FechaFin"/>
+    <tableColumn id="5" name="TipoFin"/>
+    <tableColumn id="6" name="CantidadNivelesCorrectos"/>
+    <tableColumn id="7" name="PesoTorreFila"/>
+    <tableColumn id="8" name="PesoTorreProducto"/>
+    <tableColumn id="9" name="Lote"/>
+    <tableColumn id="10" name="TiempoTotal"/>
+  </tableColumns>
+  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="TablaCiclos_Panecillos_de_avena" displayName="TablaCiclos_Panecillos_de_avena" ref="A113:J114" headerRowCount="1">
+  <autoFilter ref="A113:J114"/>
   <tableColumns count="10">
     <tableColumn id="1" name="IdCiclo"/>
     <tableColumn id="2" name="IdTorre"/>
@@ -797,7 +835,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J102"/>
+  <dimension ref="A1:J114"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -806,7 +844,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="17" customWidth="1" min="1" max="1"/>
-    <col width="22" customWidth="1" min="2" max="2"/>
+    <col width="26" customWidth="1" min="2" max="2"/>
     <col width="21" customWidth="1" min="3" max="3"/>
     <col width="21" customWidth="1" min="4" max="4"/>
     <col width="9" customWidth="1" min="5" max="5"/>
@@ -2676,10 +2714,228 @@
         <v>5</v>
       </c>
     </row>
+    <row r="103"/>
+    <row r="104">
+      <c r="A104" s="2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nombre: </t>
+        </is>
+      </c>
+      <c r="B104" s="2" t="inlineStr">
+        <is>
+          <t>Tarta de mousse de fresa</t>
+        </is>
+      </c>
+    </row>
+    <row r="105"/>
+    <row r="106">
+      <c r="A106" s="3" t="inlineStr">
+        <is>
+          <t>LISTA DE CICLOS</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="4" t="inlineStr">
+        <is>
+          <t>IdCiclo</t>
+        </is>
+      </c>
+      <c r="B107" s="4" t="inlineStr">
+        <is>
+          <t>IdTorre</t>
+        </is>
+      </c>
+      <c r="C107" s="4" t="inlineStr">
+        <is>
+          <t>FechaInicio</t>
+        </is>
+      </c>
+      <c r="D107" s="4" t="inlineStr">
+        <is>
+          <t>FechaFin</t>
+        </is>
+      </c>
+      <c r="E107" s="4" t="inlineStr">
+        <is>
+          <t>TipoFin</t>
+        </is>
+      </c>
+      <c r="F107" s="4" t="inlineStr">
+        <is>
+          <t>CantidadNivelesCorrectos</t>
+        </is>
+      </c>
+      <c r="G107" s="4" t="inlineStr">
+        <is>
+          <t>PesoTorreFila</t>
+        </is>
+      </c>
+      <c r="H107" s="4" t="inlineStr">
+        <is>
+          <t>PesoTorreProducto</t>
+        </is>
+      </c>
+      <c r="I107" s="4" t="inlineStr">
+        <is>
+          <t>Lote</t>
+        </is>
+      </c>
+      <c r="J107" s="4" t="inlineStr">
+        <is>
+          <t>TiempoTotal</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="n">
+        <v>18</v>
+      </c>
+      <c r="B108" t="n">
+        <v>7</v>
+      </c>
+      <c r="C108" s="5" t="n">
+        <v>45830</v>
+      </c>
+      <c r="D108" s="5" t="n">
+        <v>45839.99998842592</v>
+      </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>Urgente</t>
+        </is>
+      </c>
+      <c r="F108" t="n">
+        <v>3</v>
+      </c>
+      <c r="G108" t="n">
+        <v>250</v>
+      </c>
+      <c r="H108" t="n">
+        <v>750</v>
+      </c>
+      <c r="I108" t="inlineStr">
+        <is>
+          <t>L018</t>
+        </is>
+      </c>
+      <c r="J108" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="109"/>
+    <row r="110">
+      <c r="A110" s="2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nombre: </t>
+        </is>
+      </c>
+      <c r="B110" s="2" t="inlineStr">
+        <is>
+          <t>Panecillos de avena</t>
+        </is>
+      </c>
+    </row>
+    <row r="111"/>
+    <row r="112">
+      <c r="A112" s="3" t="inlineStr">
+        <is>
+          <t>LISTA DE CICLOS</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" s="4" t="inlineStr">
+        <is>
+          <t>IdCiclo</t>
+        </is>
+      </c>
+      <c r="B113" s="4" t="inlineStr">
+        <is>
+          <t>IdTorre</t>
+        </is>
+      </c>
+      <c r="C113" s="4" t="inlineStr">
+        <is>
+          <t>FechaInicio</t>
+        </is>
+      </c>
+      <c r="D113" s="4" t="inlineStr">
+        <is>
+          <t>FechaFin</t>
+        </is>
+      </c>
+      <c r="E113" s="4" t="inlineStr">
+        <is>
+          <t>TipoFin</t>
+        </is>
+      </c>
+      <c r="F113" s="4" t="inlineStr">
+        <is>
+          <t>CantidadNivelesCorrectos</t>
+        </is>
+      </c>
+      <c r="G113" s="4" t="inlineStr">
+        <is>
+          <t>PesoTorreFila</t>
+        </is>
+      </c>
+      <c r="H113" s="4" t="inlineStr">
+        <is>
+          <t>PesoTorreProducto</t>
+        </is>
+      </c>
+      <c r="I113" s="4" t="inlineStr">
+        <is>
+          <t>Lote</t>
+        </is>
+      </c>
+      <c r="J113" s="4" t="inlineStr">
+        <is>
+          <t>TiempoTotal</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="n">
+        <v>19</v>
+      </c>
+      <c r="B114" t="n">
+        <v>8</v>
+      </c>
+      <c r="C114" s="5" t="n">
+        <v>45840</v>
+      </c>
+      <c r="D114" s="5" t="n">
+        <v>45849.99998842592</v>
+      </c>
+      <c r="E114" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="F114" t="n">
+        <v>2</v>
+      </c>
+      <c r="G114" t="n">
+        <v>70</v>
+      </c>
+      <c r="H114" t="n">
+        <v>140</v>
+      </c>
+      <c r="I114" t="inlineStr">
+        <is>
+          <t>L019</t>
+        </is>
+      </c>
+      <c r="J114" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-  <tableParts count="17">
+  <tableParts count="19">
     <tablePart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
     <tablePart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
     <tablePart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
@@ -2697,6 +2953,8 @@
     <tablePart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId16"/>
     <tablePart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId17"/>
     <tablePart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId18"/>
+    <tablePart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId19"/>
+    <tablePart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId20"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>